<commit_message>
Edit create levels from txt file and add more levels
</commit_message>
<xml_diff>
--- a/Data_Levels/levels_db.xlsx
+++ b/Data_Levels/levels_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\M_Godot\Projects\Fill_Mazes\godot_fill_mazes\Data_Levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F25905-5E15-45A2-8FFC-E2364A2EB61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1E80F8-A85C-4036-AB9F-D7A862CEAC83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8C593F1F-304C-4F25-BBD7-4659C735E401}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{8C593F1F-304C-4F25-BBD7-4659C735E401}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Row</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>Number of Generated Levels</t>
+  </si>
+  <si>
+    <t>Number of levels in game</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Level From</t>
+  </si>
+  <si>
+    <t>Level To</t>
   </si>
 </sst>
 </file>
@@ -406,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540E0933-0E28-4CCE-B48D-66A6CBD6D8DD}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,10 +429,13 @@
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,33 +448,63 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -473,7 +518,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -486,8 +531,17 @@
       <c r="D8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -501,7 +555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -515,7 +569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -529,7 +583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -542,8 +596,17 @@
       <c r="D12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -556,8 +619,17 @@
       <c r="D13">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -570,8 +642,20 @@
       <c r="D14">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>6</v>
+      </c>
+      <c r="H14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -584,8 +668,11 @@
       <c r="D15">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -596,6 +683,9 @@
         <v>15</v>
       </c>
       <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update level and hint
</commit_message>
<xml_diff>
--- a/Data_Levels/levels_db.xlsx
+++ b/Data_Levels/levels_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Godot\Fill_Mazes\godot_fill_mazes\Data_Levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81A8A29-46B8-4371-AB8F-D595C03AAEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5224EDF-9E18-4969-AB6F-8766FB789A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31110" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{8C593F1F-304C-4F25-BBD7-4659C735E401}"/>
   </bookViews>
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540E0933-0E28-4CCE-B48D-66A6CBD6D8DD}">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,7 +1122,9 @@
       <c r="C32" s="2">
         <v>31</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2">
+        <v>2716</v>
+      </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>

</xml_diff>

<commit_message>
Add more to levels db
</commit_message>
<xml_diff>
--- a/Data_Levels/levels_db.xlsx
+++ b/Data_Levels/levels_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Godot\Fill_Mazes\godot_fill_mazes\Data_Levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5224EDF-9E18-4969-AB6F-8766FB789A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779B889B-CB55-421F-BCDF-064CB56DA4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31110" yWindow="2415" windowWidth="21600" windowHeight="11385" xr2:uid="{8C593F1F-304C-4F25-BBD7-4659C735E401}"/>
   </bookViews>
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540E0933-0E28-4CCE-B48D-66A6CBD6D8DD}">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1260,9 @@
       <c r="C40" s="2">
         <v>39</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="D40" s="2">
+        <v>74</v>
+      </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>

</xml_diff>

<commit_message>
Edited and add more levels
</commit_message>
<xml_diff>
--- a/Data_Levels/levels_db.xlsx
+++ b/Data_Levels/levels_db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Godot\Fill_Mazes\godot_fill_mazes\Data_Levels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\M_Godot\Projects\Fill_Mazes\godot_fill_mazes\Data_Levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247DD836-CC0F-48CE-87FB-01AAE1DFF88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EEB8A7-50AB-46E9-A024-884B21614E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{8C593F1F-304C-4F25-BBD7-4659C735E401}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{8C593F1F-304C-4F25-BBD7-4659C735E401}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Row</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>Level To</t>
+  </si>
+  <si>
+    <t>Zoom</t>
+  </si>
+  <si>
+    <t>4 x 5</t>
+  </si>
+  <si>
+    <t>5 x 6</t>
+  </si>
+  <si>
+    <t>6 x 7</t>
   </si>
 </sst>
 </file>
@@ -101,10 +113,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,24 +447,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540E0933-0E28-4CCE-B48D-66A6CBD6D8DD}">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -461,8 +489,11 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2">
@@ -473,8 +504,9 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2">
@@ -485,8 +517,9 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2">
@@ -503,8 +536,11 @@
         <v>1</v>
       </c>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="4">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
@@ -515,8 +551,9 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2">
@@ -533,8 +570,9 @@
         <v>2</v>
       </c>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -551,8 +589,9 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -575,26 +614,28 @@
         <v>3</v>
       </c>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>3</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="5">
         <v>3</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="5">
         <v>8</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="5">
         <v>0</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>3</v>
       </c>
@@ -611,8 +652,9 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -629,8 +671,9 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -653,8 +696,9 @@
         <v>4</v>
       </c>
       <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>4</v>
       </c>
@@ -677,8 +721,9 @@
         <v>5</v>
       </c>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>4</v>
       </c>
@@ -703,8 +748,9 @@
       <c r="H14" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>4</v>
       </c>
@@ -729,8 +775,9 @@
       <c r="H15" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>4</v>
       </c>
@@ -753,8 +800,9 @@
         <v>18</v>
       </c>
       <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -779,8 +827,11 @@
       <c r="H17" s="2">
         <v>58</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>4</v>
       </c>
@@ -805,8 +856,9 @@
       <c r="H18" s="2">
         <v>108</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>4</v>
       </c>
@@ -831,8 +883,9 @@
       <c r="H19" s="2">
         <v>118</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>4</v>
       </c>
@@ -855,8 +908,9 @@
         <v>119</v>
       </c>
       <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>5</v>
       </c>
@@ -881,8 +935,9 @@
       <c r="H21" s="2">
         <v>200</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>5</v>
       </c>
@@ -907,8 +962,9 @@
       <c r="H22" s="2">
         <v>300</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>5</v>
       </c>
@@ -933,8 +989,9 @@
       <c r="H23" s="2">
         <v>37</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>5</v>
       </c>
@@ -959,26 +1016,28 @@
       <c r="H24" s="2">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1">
-        <v>5</v>
-      </c>
-      <c r="C25" s="1">
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>5</v>
+      </c>
+      <c r="B25" s="5">
+        <v>5</v>
+      </c>
+      <c r="C25" s="5">
         <v>24</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="5">
         <v>0</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>5</v>
       </c>
@@ -1003,8 +1062,9 @@
       <c r="H26" s="2">
         <v>300</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>5</v>
       </c>
@@ -1025,8 +1085,9 @@
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>5</v>
       </c>
@@ -1051,8 +1112,9 @@
       <c r="H28" s="2">
         <v>89</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>5</v>
       </c>
@@ -1077,26 +1139,28 @@
       <c r="H29" s="2">
         <v>91</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>5</v>
-      </c>
-      <c r="B30" s="1">
-        <v>6</v>
-      </c>
-      <c r="C30" s="1">
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>5</v>
+      </c>
+      <c r="B30" s="5">
+        <v>6</v>
+      </c>
+      <c r="C30" s="5">
         <v>29</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="5">
         <v>0</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>6</v>
       </c>
@@ -1109,12 +1173,23 @@
       <c r="D31" s="2">
         <v>10031</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E31" s="2">
+        <v>300</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="2">
+        <v>92</v>
+      </c>
+      <c r="H31" s="2">
+        <v>91</v>
+      </c>
+      <c r="I31" s="6">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>6</v>
       </c>
@@ -1127,12 +1202,21 @@
       <c r="D32" s="2">
         <v>2716</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E32" s="2">
+        <v>371</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" s="2">
+        <v>92</v>
+      </c>
+      <c r="H32" s="2">
+        <v>162</v>
+      </c>
+      <c r="I32" s="6"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>6</v>
       </c>
@@ -1145,12 +1229,21 @@
       <c r="D33" s="2">
         <v>370</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E33" s="2">
+        <v>370</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="2">
+        <v>163</v>
+      </c>
+      <c r="H33" s="2">
+        <v>232</v>
+      </c>
+      <c r="I33" s="6"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>6</v>
       </c>
@@ -1163,48 +1256,59 @@
       <c r="D34" s="2">
         <v>68</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>6</v>
-      </c>
-      <c r="B35" s="1">
-        <v>6</v>
-      </c>
-      <c r="C35" s="1">
+      <c r="E34" s="2">
+        <v>68</v>
+      </c>
+      <c r="F34" s="2">
+        <v>7</v>
+      </c>
+      <c r="G34" s="2">
+        <v>233</v>
+      </c>
+      <c r="H34" s="2">
+        <v>300</v>
+      </c>
+      <c r="I34" s="6"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>6</v>
+      </c>
+      <c r="B35" s="5">
+        <v>6</v>
+      </c>
+      <c r="C35" s="5">
         <v>34</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="5">
         <v>0</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>6</v>
-      </c>
-      <c r="B36" s="1">
-        <v>6</v>
-      </c>
-      <c r="C36" s="1">
+      <c r="I35" s="6"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>6</v>
+      </c>
+      <c r="B36" s="5">
+        <v>6</v>
+      </c>
+      <c r="C36" s="5">
         <v>35</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="5">
         <v>0</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="6"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>6</v>
       </c>
@@ -1219,8 +1323,9 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="6"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>6</v>
       </c>
@@ -1235,8 +1340,9 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="6"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>6</v>
       </c>
@@ -1251,8 +1357,9 @@
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="6"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>6</v>
       </c>
@@ -1267,44 +1374,47 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>6</v>
-      </c>
-      <c r="B41" s="1">
-        <v>7</v>
-      </c>
-      <c r="C41" s="1">
+      <c r="I40" s="6"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>6</v>
+      </c>
+      <c r="B41" s="5">
+        <v>7</v>
+      </c>
+      <c r="C41" s="5">
         <v>40</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="5">
         <v>0</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>6</v>
-      </c>
-      <c r="B42" s="1">
-        <v>7</v>
-      </c>
-      <c r="C42" s="1">
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>6</v>
+      </c>
+      <c r="B42" s="5">
+        <v>7</v>
+      </c>
+      <c r="C42" s="5">
         <v>41</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="5">
         <v>0</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="6"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>7</v>
       </c>
@@ -1319,8 +1429,9 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>7</v>
       </c>
@@ -1335,8 +1446,9 @@
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>7</v>
       </c>
@@ -1351,8 +1463,9 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>7</v>
       </c>
@@ -1367,8 +1480,9 @@
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>7</v>
       </c>
@@ -1383,8 +1497,9 @@
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>7</v>
       </c>
@@ -1399,8 +1514,9 @@
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>7</v>
       </c>
@@ -1415,8 +1531,9 @@
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2">
@@ -1427,8 +1544,9 @@
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="3"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2">
@@ -1439,8 +1557,9 @@
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="3"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2">
@@ -1451,8 +1570,9 @@
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2">
@@ -1463,8 +1583,9 @@
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2">
@@ -1475,8 +1596,9 @@
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2">
@@ -1487,8 +1609,9 @@
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="3"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2">
@@ -1499,8 +1622,9 @@
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="3"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2">
@@ -1511,8 +1635,9 @@
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="3"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2">
@@ -1523,8 +1648,9 @@
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="3"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2">
@@ -1535,8 +1661,9 @@
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="3"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2">
@@ -1547,8 +1674,9 @@
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="3"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2">
@@ -1559,8 +1687,9 @@
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="3"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2">
@@ -1571,8 +1700,9 @@
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="3"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2">
@@ -1583,8 +1713,9 @@
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="3"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2">
@@ -1595,8 +1726,9 @@
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="3"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2">
@@ -1607,8 +1739,9 @@
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="3"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2">
@@ -1619,8 +1752,9 @@
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="3"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2">
@@ -1631,8 +1765,9 @@
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="3"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2">
@@ -1643,8 +1778,9 @@
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="3"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2">
@@ -1655,8 +1791,9 @@
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="3"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2">
@@ -1667,8 +1804,9 @@
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="3"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2">
@@ -1679,8 +1817,9 @@
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="3"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2">
@@ -1691,8 +1830,9 @@
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2">
@@ -1703,8 +1843,9 @@
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="3"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2">
@@ -1715,8 +1856,9 @@
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="3"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2">
@@ -1727,8 +1869,9 @@
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="3"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2">
@@ -1739,8 +1882,9 @@
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="3"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2">
@@ -1751,8 +1895,9 @@
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="3"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2">
@@ -1763,8 +1908,9 @@
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="3"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2">
@@ -1775,8 +1921,9 @@
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="3"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2">
@@ -1787,8 +1934,9 @@
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="3"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2">
@@ -1799,8 +1947,14 @@
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
+      <c r="I81" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I4:I16"/>
+    <mergeCell ref="I17:I30"/>
+    <mergeCell ref="I31:I42"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added to levels db
</commit_message>
<xml_diff>
--- a/Data_Levels/levels_db.xlsx
+++ b/Data_Levels/levels_db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\M_Godot\Projects\Fill_Mazes\godot_fill_mazes\Data_Levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EEB8A7-50AB-46E9-A024-884B21614E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD821B6-0CB4-4EDF-8DC5-060F2B744BBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{8C593F1F-304C-4F25-BBD7-4659C735E401}"/>
   </bookViews>
@@ -124,10 +124,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -449,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540E0933-0E28-4CCE-B48D-66A6CBD6D8DD}">
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +536,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="2"/>
-      <c r="I4" s="4">
+      <c r="I4" s="5">
         <v>0.65</v>
       </c>
     </row>
@@ -551,7 +551,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="4"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -570,7 +570,7 @@
         <v>2</v>
       </c>
       <c r="H6" s="2"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -589,7 +589,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="4"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -614,26 +614,26 @@
         <v>3</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>3</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>3</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>8</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>0</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="4"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -652,7 +652,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="4"/>
+      <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -671,7 +671,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="4"/>
+      <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -696,7 +696,7 @@
         <v>4</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="4"/>
+      <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -721,7 +721,7 @@
         <v>5</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="4"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -748,7 +748,7 @@
       <c r="H14" s="2">
         <v>13</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -775,7 +775,7 @@
       <c r="H15" s="2">
         <v>17</v>
       </c>
-      <c r="I15" s="4"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -800,7 +800,7 @@
         <v>18</v>
       </c>
       <c r="H16" s="2"/>
-      <c r="I16" s="4"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -827,7 +827,7 @@
       <c r="H17" s="2">
         <v>58</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="5">
         <v>0.75</v>
       </c>
     </row>
@@ -856,7 +856,7 @@
       <c r="H18" s="2">
         <v>108</v>
       </c>
-      <c r="I18" s="4"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
@@ -883,7 +883,7 @@
       <c r="H19" s="2">
         <v>118</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
@@ -908,7 +908,7 @@
         <v>119</v>
       </c>
       <c r="H20" s="2"/>
-      <c r="I20" s="4"/>
+      <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
@@ -935,7 +935,7 @@
       <c r="H21" s="2">
         <v>200</v>
       </c>
-      <c r="I21" s="4"/>
+      <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
@@ -962,7 +962,7 @@
       <c r="H22" s="2">
         <v>300</v>
       </c>
-      <c r="I22" s="4"/>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -989,7 +989,7 @@
       <c r="H23" s="2">
         <v>37</v>
       </c>
-      <c r="I23" s="4"/>
+      <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
@@ -1016,26 +1016,26 @@
       <c r="H24" s="2">
         <v>42</v>
       </c>
-      <c r="I24" s="4"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>5</v>
-      </c>
-      <c r="B25" s="5">
-        <v>5</v>
-      </c>
-      <c r="C25" s="5">
+      <c r="A25" s="4">
+        <v>5</v>
+      </c>
+      <c r="B25" s="4">
+        <v>5</v>
+      </c>
+      <c r="C25" s="4">
         <v>24</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>0</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="4"/>
+      <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
@@ -1062,7 +1062,7 @@
       <c r="H26" s="2">
         <v>300</v>
       </c>
-      <c r="I26" s="4"/>
+      <c r="I26" s="5"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -1085,7 +1085,7 @@
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="4"/>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -1112,7 +1112,7 @@
       <c r="H28" s="2">
         <v>89</v>
       </c>
-      <c r="I28" s="4"/>
+      <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -1139,26 +1139,26 @@
       <c r="H29" s="2">
         <v>91</v>
       </c>
-      <c r="I29" s="4"/>
+      <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
-        <v>5</v>
-      </c>
-      <c r="B30" s="5">
-        <v>6</v>
-      </c>
-      <c r="C30" s="5">
+      <c r="A30" s="4">
+        <v>5</v>
+      </c>
+      <c r="B30" s="4">
+        <v>6</v>
+      </c>
+      <c r="C30" s="4">
         <v>29</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="4">
         <v>0</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="4"/>
+      <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
@@ -1271,16 +1271,16 @@
       <c r="I34" s="6"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>6</v>
-      </c>
-      <c r="B35" s="5">
-        <v>6</v>
-      </c>
-      <c r="C35" s="5">
+      <c r="A35" s="4">
+        <v>6</v>
+      </c>
+      <c r="B35" s="4">
+        <v>6</v>
+      </c>
+      <c r="C35" s="4">
         <v>34</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="4">
         <v>0</v>
       </c>
       <c r="E35" s="2"/>
@@ -1290,16 +1290,16 @@
       <c r="I35" s="6"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
-        <v>6</v>
-      </c>
-      <c r="B36" s="5">
-        <v>6</v>
-      </c>
-      <c r="C36" s="5">
+      <c r="A36" s="4">
+        <v>6</v>
+      </c>
+      <c r="B36" s="4">
+        <v>6</v>
+      </c>
+      <c r="C36" s="4">
         <v>35</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="4">
         <v>0</v>
       </c>
       <c r="E36" s="2"/>
@@ -1369,7 +1369,9 @@
       <c r="C40" s="2">
         <v>39</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="D40" s="2">
+        <v>74</v>
+      </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -1377,16 +1379,16 @@
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
-        <v>6</v>
-      </c>
-      <c r="B41" s="5">
-        <v>7</v>
-      </c>
-      <c r="C41" s="5">
+      <c r="A41" s="4">
+        <v>6</v>
+      </c>
+      <c r="B41" s="4">
+        <v>7</v>
+      </c>
+      <c r="C41" s="4">
         <v>40</v>
       </c>
-      <c r="D41" s="5">
+      <c r="D41" s="4">
         <v>0</v>
       </c>
       <c r="E41" s="2"/>
@@ -1396,16 +1398,16 @@
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
-        <v>6</v>
-      </c>
-      <c r="B42" s="5">
-        <v>7</v>
-      </c>
-      <c r="C42" s="5">
+      <c r="A42" s="4">
+        <v>6</v>
+      </c>
+      <c r="B42" s="4">
+        <v>7</v>
+      </c>
+      <c r="C42" s="4">
         <v>41</v>
       </c>
-      <c r="D42" s="5">
+      <c r="D42" s="4">
         <v>0</v>
       </c>
       <c r="E42" s="2"/>
@@ -1517,21 +1519,23 @@
       <c r="I48" s="3"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>7</v>
-      </c>
-      <c r="B49" s="2">
-        <v>7</v>
-      </c>
-      <c r="C49" s="2">
+      <c r="A49" s="4">
+        <v>7</v>
+      </c>
+      <c r="B49" s="4">
+        <v>7</v>
+      </c>
+      <c r="C49" s="4">
         <v>48</v>
       </c>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="3"/>
+      <c r="D49" s="4">
+        <v>0</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>

</xml_diff>